<commit_message>
Frame Counts 1 word Excel Sheet added
</commit_message>
<xml_diff>
--- a/Dataset Excel Sheets/frames_counts_1word.xlsx
+++ b/Dataset Excel Sheets/frames_counts_1word.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/080c280c8b6910c1/Desktop/AUS/4. Senior Year/Spring 2024/Senior Design II/Senior-Design-Code/Dataset Excel Sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salma\Desktop\Senior Design\CSE 491 - Senior Design II\github\Senior-Design-Code\Dataset Excel Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_6D4DD4975BE0537293983B11595ED87656C92A4B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E6C15C6-F99E-4F6B-AEB8-602328782308}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD0145B-7A8B-40EE-96A0-8E52B726F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="252" yWindow="60" windowWidth="22212" windowHeight="13428" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$B$2281</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -6886,12 +6889,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -6921,11 +6930,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7230,8 +7240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A946" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7273,10 +7283,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>9</v>
       </c>
     </row>
@@ -7369,18 +7379,18 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>0</v>
       </c>
     </row>
@@ -7521,10 +7531,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="2">
         <v>61</v>
       </c>
     </row>
@@ -7585,18 +7595,18 @@
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="2">
         <v>28</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="2">
         <v>86</v>
       </c>
     </row>
@@ -8177,10 +8187,10 @@
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+      <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="2">
         <v>89</v>
       </c>
     </row>
@@ -8537,10 +8547,10 @@
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" t="s">
+      <c r="A163" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B163">
+      <c r="B163" s="2">
         <v>4</v>
       </c>
     </row>
@@ -8665,10 +8675,10 @@
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" t="s">
+      <c r="A179" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="B179">
+      <c r="B179" s="2">
         <v>74</v>
       </c>
     </row>
@@ -9121,10 +9131,10 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" t="s">
+      <c r="A236" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B236">
+      <c r="B236" s="2">
         <v>23</v>
       </c>
     </row>
@@ -9945,10 +9955,10 @@
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A339" t="s">
+      <c r="A339" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B339">
+      <c r="B339" s="2">
         <v>97</v>
       </c>
     </row>
@@ -10321,10 +10331,10 @@
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A386" t="s">
+      <c r="A386" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="B386">
+      <c r="B386" s="2">
         <v>4</v>
       </c>
     </row>
@@ -10489,10 +10499,10 @@
       </c>
     </row>
     <row r="407" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A407" t="s">
+      <c r="A407" s="2" t="s">
         <v>406</v>
       </c>
-      <c r="B407">
+      <c r="B407" s="2">
         <v>9</v>
       </c>
     </row>
@@ -10561,10 +10571,10 @@
       </c>
     </row>
     <row r="416" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A416" t="s">
+      <c r="A416" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="B416">
+      <c r="B416" s="2">
         <v>63</v>
       </c>
     </row>
@@ -10913,10 +10923,10 @@
       </c>
     </row>
     <row r="460" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A460" t="s">
+      <c r="A460" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B460">
+      <c r="B460" s="2">
         <v>66</v>
       </c>
     </row>
@@ -10977,10 +10987,10 @@
       </c>
     </row>
     <row r="468" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A468" t="s">
+      <c r="A468" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B468">
+      <c r="B468" s="2">
         <v>69</v>
       </c>
     </row>
@@ -11425,10 +11435,10 @@
       </c>
     </row>
     <row r="524" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A524" t="s">
+      <c r="A524" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="B524">
+      <c r="B524" s="2">
         <v>96</v>
       </c>
     </row>
@@ -11745,10 +11755,10 @@
       </c>
     </row>
     <row r="564" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A564" t="s">
+      <c r="A564" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B564">
+      <c r="B564" s="2">
         <v>14</v>
       </c>
     </row>
@@ -12481,10 +12491,10 @@
       </c>
     </row>
     <row r="656" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A656" t="s">
+      <c r="A656" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="B656">
+      <c r="B656" s="2">
         <v>19</v>
       </c>
     </row>
@@ -12689,10 +12699,10 @@
       </c>
     </row>
     <row r="682" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A682" t="s">
+      <c r="A682" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="B682">
+      <c r="B682" s="2">
         <v>55</v>
       </c>
     </row>
@@ -13209,10 +13219,10 @@
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A747" t="s">
+      <c r="A747" s="2" t="s">
         <v>746</v>
       </c>
-      <c r="B747">
+      <c r="B747" s="2">
         <v>0</v>
       </c>
     </row>
@@ -13233,10 +13243,10 @@
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A750" t="s">
+      <c r="A750" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="B750">
+      <c r="B750" s="2">
         <v>45</v>
       </c>
     </row>
@@ -13393,10 +13403,10 @@
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A770" t="s">
+      <c r="A770" s="2" t="s">
         <v>769</v>
       </c>
-      <c r="B770">
+      <c r="B770" s="2">
         <v>90</v>
       </c>
     </row>
@@ -13729,10 +13739,10 @@
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A812" t="s">
+      <c r="A812" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="B812">
+      <c r="B812" s="2">
         <v>2</v>
       </c>
     </row>
@@ -14105,10 +14115,10 @@
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A859" t="s">
+      <c r="A859" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="B859">
+      <c r="B859" s="2">
         <v>85</v>
       </c>
     </row>
@@ -15265,10 +15275,10 @@
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1004" t="s">
+      <c r="A1004" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="B1004">
+      <c r="B1004" s="2">
         <v>1</v>
       </c>
     </row>
@@ -15433,10 +15443,10 @@
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1025" t="s">
+      <c r="A1025" s="2" t="s">
         <v>1024</v>
       </c>
-      <c r="B1025">
+      <c r="B1025" s="2">
         <v>86</v>
       </c>
     </row>
@@ -15897,10 +15907,10 @@
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1083" t="s">
+      <c r="A1083" s="2" t="s">
         <v>1082</v>
       </c>
-      <c r="B1083">
+      <c r="B1083" s="2">
         <v>96</v>
       </c>
     </row>
@@ -16497,10 +16507,10 @@
       </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1158" t="s">
+      <c r="A1158" s="2" t="s">
         <v>1157</v>
       </c>
-      <c r="B1158">
+      <c r="B1158" s="2">
         <v>0</v>
       </c>
     </row>
@@ -17017,10 +17027,10 @@
       </c>
     </row>
     <row r="1223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1223" t="s">
+      <c r="A1223" s="2" t="s">
         <v>1222</v>
       </c>
-      <c r="B1223">
+      <c r="B1223" s="2">
         <v>0</v>
       </c>
     </row>
@@ -17057,10 +17067,10 @@
       </c>
     </row>
     <row r="1228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1228" t="s">
+      <c r="A1228" s="2" t="s">
         <v>1227</v>
       </c>
-      <c r="B1228">
+      <c r="B1228" s="2">
         <v>75</v>
       </c>
     </row>
@@ -17945,10 +17955,10 @@
       </c>
     </row>
     <row r="1339" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1339" t="s">
+      <c r="A1339" s="2" t="s">
         <v>1338</v>
       </c>
-      <c r="B1339">
+      <c r="B1339" s="2">
         <v>47</v>
       </c>
     </row>
@@ -18681,10 +18691,10 @@
       </c>
     </row>
     <row r="1431" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1431" t="s">
+      <c r="A1431" s="2" t="s">
         <v>1430</v>
       </c>
-      <c r="B1431">
+      <c r="B1431" s="2">
         <v>14</v>
       </c>
     </row>
@@ -18721,10 +18731,10 @@
       </c>
     </row>
     <row r="1436" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1436" t="s">
+      <c r="A1436" s="2" t="s">
         <v>1435</v>
       </c>
-      <c r="B1436">
+      <c r="B1436" s="2">
         <v>54</v>
       </c>
     </row>
@@ -19241,10 +19251,10 @@
       </c>
     </row>
     <row r="1501" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1501" t="s">
+      <c r="A1501" s="2" t="s">
         <v>1500</v>
       </c>
-      <c r="B1501">
+      <c r="B1501" s="2">
         <v>87</v>
       </c>
     </row>
@@ -19457,18 +19467,18 @@
       </c>
     </row>
     <row r="1528" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1528" t="s">
+      <c r="A1528" s="2" t="s">
         <v>1527</v>
       </c>
-      <c r="B1528">
+      <c r="B1528" s="2">
         <v>82</v>
       </c>
     </row>
     <row r="1529" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1529" t="s">
+      <c r="A1529" s="2" t="s">
         <v>1528</v>
       </c>
-      <c r="B1529">
+      <c r="B1529" s="2">
         <v>49</v>
       </c>
     </row>
@@ -19505,10 +19515,10 @@
       </c>
     </row>
     <row r="1534" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1534" t="s">
+      <c r="A1534" s="2" t="s">
         <v>1533</v>
       </c>
-      <c r="B1534">
+      <c r="B1534" s="2">
         <v>58</v>
       </c>
     </row>
@@ -20025,10 +20035,10 @@
       </c>
     </row>
     <row r="1599" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1599" t="s">
+      <c r="A1599" s="2" t="s">
         <v>1598</v>
       </c>
-      <c r="B1599">
+      <c r="B1599" s="2">
         <v>65</v>
       </c>
     </row>
@@ -20201,18 +20211,18 @@
       </c>
     </row>
     <row r="1621" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1621" t="s">
+      <c r="A1621" s="2" t="s">
         <v>1620</v>
       </c>
-      <c r="B1621">
+      <c r="B1621" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="1622" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1622" t="s">
+      <c r="A1622" s="2" t="s">
         <v>1621</v>
       </c>
-      <c r="B1622">
+      <c r="B1622" s="2">
         <v>0</v>
       </c>
     </row>
@@ -20257,10 +20267,10 @@
       </c>
     </row>
     <row r="1628" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1628" t="s">
+      <c r="A1628" s="2" t="s">
         <v>1627</v>
       </c>
-      <c r="B1628">
+      <c r="B1628" s="2">
         <v>0</v>
       </c>
     </row>
@@ -21353,10 +21363,10 @@
       </c>
     </row>
     <row r="1765" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1765" t="s">
+      <c r="A1765" s="2" t="s">
         <v>1764</v>
       </c>
-      <c r="B1765">
+      <c r="B1765" s="2">
         <v>66</v>
       </c>
     </row>
@@ -21769,10 +21779,10 @@
       </c>
     </row>
     <row r="1817" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1817" t="s">
+      <c r="A1817" s="2" t="s">
         <v>1816</v>
       </c>
-      <c r="B1817">
+      <c r="B1817" s="2">
         <v>87</v>
       </c>
     </row>
@@ -22201,10 +22211,10 @@
       </c>
     </row>
     <row r="1871" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1871" t="s">
+      <c r="A1871" s="2" t="s">
         <v>1870</v>
       </c>
-      <c r="B1871">
+      <c r="B1871" s="2">
         <v>8</v>
       </c>
     </row>
@@ -22913,10 +22923,10 @@
       </c>
     </row>
     <row r="1960" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1960" t="s">
+      <c r="A1960" s="2" t="s">
         <v>1959</v>
       </c>
-      <c r="B1960">
+      <c r="B1960" s="2">
         <v>0</v>
       </c>
     </row>
@@ -23505,10 +23515,10 @@
       </c>
     </row>
     <row r="2034" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2034" t="s">
+      <c r="A2034" s="2" t="s">
         <v>2033</v>
       </c>
-      <c r="B2034">
+      <c r="B2034" s="2">
         <v>51</v>
       </c>
     </row>
@@ -23697,10 +23707,10 @@
       </c>
     </row>
     <row r="2058" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2058" t="s">
+      <c r="A2058" s="2" t="s">
         <v>2057</v>
       </c>
-      <c r="B2058">
+      <c r="B2058" s="2">
         <v>64</v>
       </c>
     </row>
@@ -23889,10 +23899,10 @@
       </c>
     </row>
     <row r="2082" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2082" t="s">
+      <c r="A2082" s="2" t="s">
         <v>2081</v>
       </c>
-      <c r="B2082">
+      <c r="B2082" s="2">
         <v>61</v>
       </c>
     </row>
@@ -24233,10 +24243,10 @@
       </c>
     </row>
     <row r="2125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2125" t="s">
+      <c r="A2125" s="2" t="s">
         <v>2124</v>
       </c>
-      <c r="B2125">
+      <c r="B2125" s="2">
         <v>0</v>
       </c>
     </row>
@@ -24593,10 +24603,10 @@
       </c>
     </row>
     <row r="2170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2170" t="s">
+      <c r="A2170" s="2" t="s">
         <v>2169</v>
       </c>
-      <c r="B2170">
+      <c r="B2170" s="2">
         <v>30</v>
       </c>
     </row>
@@ -25185,10 +25195,10 @@
       </c>
     </row>
     <row r="2244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2244" t="s">
+      <c r="A2244" s="2" t="s">
         <v>2243</v>
       </c>
-      <c r="B2244">
+      <c r="B2244" s="2">
         <v>13</v>
       </c>
     </row>
@@ -25225,10 +25235,10 @@
       </c>
     </row>
     <row r="2249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2249" t="s">
+      <c r="A2249" s="2" t="s">
         <v>2248</v>
       </c>
-      <c r="B2249">
+      <c r="B2249" s="2">
         <v>3</v>
       </c>
     </row>
@@ -25353,10 +25363,10 @@
       </c>
     </row>
     <row r="2265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2265" t="s">
+      <c r="A2265" s="2" t="s">
         <v>2264</v>
       </c>
-      <c r="B2265">
+      <c r="B2265" s="2">
         <v>99</v>
       </c>
     </row>
@@ -25489,6 +25499,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B2281" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>